<commit_message>
a rule ctf,enum. no wirte wp yet ,should be one.
</commit_message>
<xml_diff>
--- a/oscp_like_machine_list.xlsx
+++ b/oscp_like_machine_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qianenzhao\bamuwe.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500D719B-214F-479B-88A3-48CC23737FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B838C63-EA73-4023-AA88-5D2B36CC2822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,724 +141,726 @@
     <t>Steel Mountain</t>
   </si>
   <si>
+    <t>SQL Injection Lab</t>
+  </si>
+  <si>
+    <t>Nibbles</t>
+  </si>
+  <si>
+    <t>Netmon</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>Year of the Owl</t>
+  </si>
+  <si>
+    <t>Attacking Kerberos</t>
+  </si>
+  <si>
+    <t>Linux Privilege Escalation</t>
+  </si>
+  <si>
+    <t>Solidstate</t>
+  </si>
+  <si>
+    <t>Servmon</t>
+  </si>
+  <si>
+    <t>Sauna</t>
+  </si>
+  <si>
+    <t>Kenobi</t>
+  </si>
+  <si>
+    <t>Retro</t>
+  </si>
+  <si>
+    <t>Wreath Network</t>
+  </si>
+  <si>
+    <t>Windows Privilege Escalation</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>Chatterbox</t>
+  </si>
+  <si>
+    <t>Monteverde</t>
+  </si>
+  <si>
+    <t>GameZone</t>
+  </si>
+  <si>
+    <t>Alfred</t>
+  </si>
+  <si>
+    <t>Git Happens</t>
+  </si>
+  <si>
+    <t>Knife</t>
+  </si>
+  <si>
+    <t>Jeeves</t>
+  </si>
+  <si>
+    <t>Timelapse</t>
+  </si>
+  <si>
+    <t>Skynet</t>
+  </si>
+  <si>
+    <t>Relevant</t>
+  </si>
+  <si>
+    <t>NahamStore</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Sniper</t>
+  </si>
+  <si>
+    <t>Flight</t>
+  </si>
+  <si>
+    <t>Daily bugle</t>
+  </si>
+  <si>
+    <t>Blueprint</t>
+  </si>
+  <si>
+    <t>Keeper</t>
+  </si>
+  <si>
+    <t>Querier</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Lazy admin</t>
+  </si>
+  <si>
+    <t>Hackpark</t>
+  </si>
+  <si>
+    <t>Assumed Breach Scenarios:</t>
+  </si>
+  <si>
+    <t>Pilgrimage</t>
+  </si>
+  <si>
+    <t>Giddy</t>
+  </si>
+  <si>
+    <t>Blackfield</t>
+  </si>
+  <si>
+    <t>Tomghost</t>
+  </si>
+  <si>
+    <t>Weasel</t>
+  </si>
+  <si>
+    <t>Corp</t>
+  </si>
+  <si>
+    <t>Cozyhosting</t>
+  </si>
+  <si>
+    <t>Bounty</t>
+  </si>
+  <si>
+    <t>Cicada</t>
+  </si>
+  <si>
+    <t>Rootme</t>
+  </si>
+  <si>
+    <t>AllSignsPoint2Pwnage</t>
+  </si>
+  <si>
+    <t>Lateral Movement and Pivoting</t>
+  </si>
+  <si>
+    <t>Codify</t>
+  </si>
+  <si>
+    <t>Artic</t>
+  </si>
+  <si>
+    <t>Escape</t>
+  </si>
+  <si>
+    <t>CMesS</t>
+  </si>
+  <si>
+    <t>Anthem</t>
+  </si>
+  <si>
+    <t>Exploiting Active Directory</t>
+  </si>
+  <si>
+    <t>Tartarsauce</t>
+  </si>
+  <si>
+    <t>Remote</t>
+  </si>
+  <si>
+    <t>Ultratech</t>
+  </si>
+  <si>
+    <t>Jarvis</t>
+  </si>
+  <si>
+    <t>Buff</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Tabby</t>
+  </si>
+  <si>
+    <t>Love</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>Zeno</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Secnotes</t>
+  </si>
+  <si>
+    <t>Certified (harder)</t>
+  </si>
+  <si>
+    <t>Boiler CTF</t>
+  </si>
+  <si>
+    <t>Mentor</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Wonderland</t>
+  </si>
+  <si>
+    <t>Devvortex</t>
+  </si>
+  <si>
+    <t>Mailing</t>
+  </si>
+  <si>
+    <t>Silver Platter</t>
+  </si>
+  <si>
+    <t>Irked</t>
+  </si>
+  <si>
+    <t>Heist</t>
+  </si>
+  <si>
+    <t>ProLabs:</t>
+  </si>
+  <si>
+    <t>Update:</t>
+  </si>
+  <si>
+    <t>Popcorn</t>
+  </si>
+  <si>
+    <t>Dante</t>
+  </si>
+  <si>
+    <t>11/9/2024 Added Administrator to htb list, really good practice for bloodhound!</t>
+  </si>
+  <si>
+    <t>Bashed</t>
+  </si>
+  <si>
+    <t>Zephyr (harder)</t>
+  </si>
+  <si>
+    <t>11/20/2024 Acute will be replaced with Giddy in htb list</t>
+  </si>
+  <si>
+    <t>Broker</t>
+  </si>
+  <si>
+    <t>11/27/2024 Added Heist to htb list</t>
+  </si>
+  <si>
+    <t>Analytics</t>
+  </si>
+  <si>
+    <t>12/07/2024 Added Linkvortex to htb list and Reset to thm list</t>
+  </si>
+  <si>
+    <t>Networked</t>
+  </si>
+  <si>
+    <t>12/21/2024 Added UnderPass to htb list</t>
+  </si>
+  <si>
+    <t>UpDown</t>
+  </si>
+  <si>
+    <t>Swagshop</t>
+  </si>
+  <si>
+    <t>Nineveh</t>
+  </si>
+  <si>
+    <t>Pandora</t>
+  </si>
+  <si>
+    <t>OpenAdmin</t>
+  </si>
+  <si>
+    <t>Precious</t>
+  </si>
+  <si>
+    <t>Busqueda</t>
+  </si>
+  <si>
+    <t>Monitored</t>
+  </si>
+  <si>
+    <t>BoardLight</t>
+  </si>
+  <si>
+    <t>Magic</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>Editorial</t>
+  </si>
+  <si>
+    <t>Builder</t>
+  </si>
+  <si>
+    <t>Linkvortex</t>
+  </si>
+  <si>
+    <t>UnderPass</t>
+  </si>
+  <si>
+    <t>Proving Grounds Practice</t>
+  </si>
+  <si>
+    <t>Virtual Hacking Labs</t>
+  </si>
+  <si>
+    <t>The real OSCP like boxes, this is just a list with the ones that are best practice and removing the overly complicated ones that are too out of scope and those that were boxes meant to be mostly for OSEP and OSED (example Kyoto and Nara) that were in TJNull list plus adding some new ones</t>
+  </si>
+  <si>
+    <t>Very under rated platform with very OSCP like machines, people that have used it really recommend it for OSCP including me. It has been very crucial help for those that have failed attempts to be able to pass and they are good practice for standalones. Note: seems some lab purchase options are currently out of stock</t>
+  </si>
+  <si>
+    <t>Windows Active Directory</t>
+  </si>
+  <si>
+    <t>ClamAV</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Techblog</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Pelican</t>
+  </si>
+  <si>
+    <t>Resourced</t>
+  </si>
+  <si>
+    <t>Backupadmin V2</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Payday</t>
+  </si>
+  <si>
+    <t>Algernon</t>
+  </si>
+  <si>
+    <t>Nagoya</t>
+  </si>
+  <si>
+    <t>Web01-Dev V2</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Snookums</t>
+  </si>
+  <si>
+    <t>Jacko</t>
+  </si>
+  <si>
+    <t>Hokkaido</t>
+  </si>
+  <si>
+    <t>Web01-Prd V2</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Bratarina</t>
+  </si>
+  <si>
+    <t>Craft</t>
+  </si>
+  <si>
+    <t>Hutch</t>
+  </si>
+  <si>
+    <t>Forum</t>
+  </si>
+  <si>
+    <t>WinAS01</t>
+  </si>
+  <si>
+    <t>Pebbles</t>
+  </si>
+  <si>
+    <t>Squid</t>
+  </si>
+  <si>
+    <t>Vault</t>
+  </si>
+  <si>
+    <t>Quick</t>
+  </si>
+  <si>
+    <t>AS45</t>
+  </si>
+  <si>
+    <t>Nickel</t>
+  </si>
+  <si>
+    <t>Tiki</t>
+  </si>
+  <si>
+    <t>Trace</t>
+  </si>
+  <si>
+    <t>Hetemit</t>
+  </si>
+  <si>
+    <t>MedJed</t>
+  </si>
+  <si>
+    <t>Helpdesk V2</t>
+  </si>
+  <si>
+    <t>React</t>
+  </si>
+  <si>
+    <t>ZenPhoto</t>
+  </si>
+  <si>
+    <t>Billyboss</t>
+  </si>
+  <si>
+    <t>VPS1723 V2</t>
+  </si>
+  <si>
+    <t>Nukem</t>
+  </si>
+  <si>
+    <t>Shenzi</t>
+  </si>
+  <si>
+    <t>CMS02 V2</t>
+  </si>
+  <si>
+    <t>Cockpit</t>
+  </si>
+  <si>
+    <t>AuthBy</t>
+  </si>
+  <si>
+    <t>Records</t>
+  </si>
+  <si>
+    <t>PyLoader</t>
+  </si>
+  <si>
+    <t>Slort</t>
+  </si>
+  <si>
+    <t>Trails</t>
+  </si>
+  <si>
+    <t>Clue</t>
+  </si>
+  <si>
+    <t>Hepet</t>
+  </si>
+  <si>
+    <t>Dolphin V2</t>
+  </si>
+  <si>
+    <t>Extplorer</t>
+  </si>
+  <si>
+    <t>DVR4</t>
+  </si>
+  <si>
+    <t>Crash</t>
+  </si>
+  <si>
+    <t>Postfish</t>
+  </si>
+  <si>
+    <t>Natural</t>
+  </si>
+  <si>
+    <t>Hawat</t>
+  </si>
+  <si>
+    <t>Mantis</t>
+  </si>
+  <si>
+    <t>Walla</t>
+  </si>
+  <si>
+    <t>Fed V2</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>CMS01</t>
+  </si>
+  <si>
+    <t>Apex</t>
+  </si>
+  <si>
+    <t>Tracking</t>
+  </si>
+  <si>
+    <t>Sorcerer</t>
+  </si>
+  <si>
+    <t>JS01</t>
+  </si>
+  <si>
+    <t>Sybaris</t>
+  </si>
+  <si>
+    <t>PBX</t>
+  </si>
+  <si>
+    <t>Peppo</t>
+  </si>
+  <si>
+    <t>Code V2</t>
+  </si>
+  <si>
+    <t>Hunit</t>
+  </si>
+  <si>
+    <t>Teamspeak</t>
+  </si>
+  <si>
+    <t>Readys</t>
+  </si>
+  <si>
+    <t>CMS101</t>
+  </si>
+  <si>
+    <t>Astronaut</t>
+  </si>
+  <si>
+    <t>FW01</t>
+  </si>
+  <si>
+    <t>Bullybox</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Websrv01</t>
+  </si>
+  <si>
+    <t>Exfiltrated</t>
+  </si>
+  <si>
+    <t>Mon02</t>
+  </si>
+  <si>
+    <t>Fanatastic</t>
+  </si>
+  <si>
+    <t>Graphs01</t>
+  </si>
+  <si>
+    <t>QuackerJack</t>
+  </si>
+  <si>
+    <t>PM V2</t>
+  </si>
+  <si>
+    <t>Wombo</t>
+  </si>
+  <si>
+    <t>Tracker</t>
+  </si>
+  <si>
+    <t>Flu</t>
+  </si>
+  <si>
+    <t>Roquefort</t>
+  </si>
+  <si>
+    <t>Levram</t>
+  </si>
+  <si>
+    <t>Mzeeav</t>
+  </si>
+  <si>
+    <t>LaVita</t>
+  </si>
+  <si>
+    <t>Xposedapi</t>
+  </si>
+  <si>
+    <t>Zipper</t>
+  </si>
+  <si>
+    <t>Ochima</t>
+  </si>
+  <si>
+    <t>Fired</t>
+  </si>
+  <si>
+    <t>Scrutiny</t>
+  </si>
+  <si>
+    <t>SPX</t>
+  </si>
+  <si>
+    <t>Vmdak</t>
+  </si>
+  <si>
+    <t>Proving Grounds Play</t>
+  </si>
+  <si>
+    <t>Mostly boxes from vulnhub hosted by offsec for free</t>
+  </si>
+  <si>
+    <t>Platform with realistic scenarios, really good for learning Windows and AD exploitation.</t>
+  </si>
+  <si>
+    <t>Amaterasu</t>
+  </si>
+  <si>
+    <t>Sync</t>
+  </si>
+  <si>
+    <t>Baby</t>
+  </si>
+  <si>
+    <t>Loly</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>Baby2</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>Build</t>
+  </si>
+  <si>
+    <t>Job2</t>
+  </si>
+  <si>
+    <t>Breach</t>
+  </si>
+  <si>
+    <t>Stapler</t>
+  </si>
+  <si>
+    <t>Phantom</t>
+  </si>
+  <si>
+    <t>BBScute</t>
+  </si>
+  <si>
+    <t>Sweep</t>
+  </si>
+  <si>
+    <t>Gaara</t>
+  </si>
+  <si>
+    <t>Blogger</t>
+  </si>
+  <si>
+    <t>Chains:</t>
+  </si>
+  <si>
+    <t>FunboxEasyEnum</t>
+  </si>
+  <si>
+    <t>Trusted</t>
+  </si>
+  <si>
+    <t>Reflection</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
+  </si>
+  <si>
+    <t>Lustrous</t>
+  </si>
+  <si>
+    <t>VulnLab</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reset</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
     <t>Attacktive Directory</t>
-  </si>
-  <si>
-    <t>SQL Injection Lab</t>
-  </si>
-  <si>
-    <t>Nibbles</t>
-  </si>
-  <si>
-    <t>Netmon</t>
-  </si>
-  <si>
-    <t>Forest</t>
-  </si>
-  <si>
-    <t>Thompson</t>
-  </si>
-  <si>
-    <t>Year of the Owl</t>
-  </si>
-  <si>
-    <t>Attacking Kerberos</t>
-  </si>
-  <si>
-    <t>Linux Privilege Escalation</t>
-  </si>
-  <si>
-    <t>Solidstate</t>
-  </si>
-  <si>
-    <t>Servmon</t>
-  </si>
-  <si>
-    <t>Sauna</t>
-  </si>
-  <si>
-    <t>Kenobi</t>
-  </si>
-  <si>
-    <t>Retro</t>
-  </si>
-  <si>
-    <t>Wreath Network</t>
-  </si>
-  <si>
-    <t>Windows Privilege Escalation</t>
-  </si>
-  <si>
-    <t>Poison</t>
-  </si>
-  <si>
-    <t>Chatterbox</t>
-  </si>
-  <si>
-    <t>Monteverde</t>
-  </si>
-  <si>
-    <t>GameZone</t>
-  </si>
-  <si>
-    <t>Alfred</t>
-  </si>
-  <si>
-    <t>Reset</t>
-  </si>
-  <si>
-    <t>Git Happens</t>
-  </si>
-  <si>
-    <t>Knife</t>
-  </si>
-  <si>
-    <t>Jeeves</t>
-  </si>
-  <si>
-    <t>Timelapse</t>
-  </si>
-  <si>
-    <t>Skynet</t>
-  </si>
-  <si>
-    <t>Relevant</t>
-  </si>
-  <si>
-    <t>NahamStore</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Sniper</t>
-  </si>
-  <si>
-    <t>Flight</t>
-  </si>
-  <si>
-    <t>Daily bugle</t>
-  </si>
-  <si>
-    <t>Blueprint</t>
-  </si>
-  <si>
-    <t>Keeper</t>
-  </si>
-  <si>
-    <t>Querier</t>
-  </si>
-  <si>
-    <t>Return</t>
-  </si>
-  <si>
-    <t>Lazy admin</t>
-  </si>
-  <si>
-    <t>Hackpark</t>
-  </si>
-  <si>
-    <t>Assumed Breach Scenarios:</t>
-  </si>
-  <si>
-    <t>Pilgrimage</t>
-  </si>
-  <si>
-    <t>Giddy</t>
-  </si>
-  <si>
-    <t>Blackfield</t>
-  </si>
-  <si>
-    <t>Tomghost</t>
-  </si>
-  <si>
-    <t>Weasel</t>
-  </si>
-  <si>
-    <t>Corp</t>
-  </si>
-  <si>
-    <t>Cozyhosting</t>
-  </si>
-  <si>
-    <t>Bounty</t>
-  </si>
-  <si>
-    <t>Cicada</t>
-  </si>
-  <si>
-    <t>Rootme</t>
-  </si>
-  <si>
-    <t>AllSignsPoint2Pwnage</t>
-  </si>
-  <si>
-    <t>Lateral Movement and Pivoting</t>
-  </si>
-  <si>
-    <t>Codify</t>
-  </si>
-  <si>
-    <t>Artic</t>
-  </si>
-  <si>
-    <t>Escape</t>
-  </si>
-  <si>
-    <t>CMesS</t>
-  </si>
-  <si>
-    <t>Anthem</t>
-  </si>
-  <si>
-    <t>Exploiting Active Directory</t>
-  </si>
-  <si>
-    <t>Tartarsauce</t>
-  </si>
-  <si>
-    <t>Remote</t>
-  </si>
-  <si>
-    <t>Ultratech</t>
-  </si>
-  <si>
-    <t>Jarvis</t>
-  </si>
-  <si>
-    <t>Buff</t>
-  </si>
-  <si>
-    <t>Internal</t>
-  </si>
-  <si>
-    <t>Tabby</t>
-  </si>
-  <si>
-    <t>Love</t>
-  </si>
-  <si>
-    <t>Administrator</t>
-  </si>
-  <si>
-    <t>Zeno</t>
-  </si>
-  <si>
-    <t>Usage</t>
-  </si>
-  <si>
-    <t>Secnotes</t>
-  </si>
-  <si>
-    <t>Certified (harder)</t>
-  </si>
-  <si>
-    <t>Boiler CTF</t>
-  </si>
-  <si>
-    <t>Mentor</t>
-  </si>
-  <si>
-    <t>Access</t>
-  </si>
-  <si>
-    <t>Wonderland</t>
-  </si>
-  <si>
-    <t>Devvortex</t>
-  </si>
-  <si>
-    <t>Mailing</t>
-  </si>
-  <si>
-    <t>Silver Platter</t>
-  </si>
-  <si>
-    <t>Irked</t>
-  </si>
-  <si>
-    <t>Heist</t>
-  </si>
-  <si>
-    <t>ProLabs:</t>
-  </si>
-  <si>
-    <t>Update:</t>
-  </si>
-  <si>
-    <t>Popcorn</t>
-  </si>
-  <si>
-    <t>Dante</t>
-  </si>
-  <si>
-    <t>11/9/2024 Added Administrator to htb list, really good practice for bloodhound!</t>
-  </si>
-  <si>
-    <t>Bashed</t>
-  </si>
-  <si>
-    <t>Zephyr (harder)</t>
-  </si>
-  <si>
-    <t>11/20/2024 Acute will be replaced with Giddy in htb list</t>
-  </si>
-  <si>
-    <t>Broker</t>
-  </si>
-  <si>
-    <t>11/27/2024 Added Heist to htb list</t>
-  </si>
-  <si>
-    <t>Analytics</t>
-  </si>
-  <si>
-    <t>12/07/2024 Added Linkvortex to htb list and Reset to thm list</t>
-  </si>
-  <si>
-    <t>Networked</t>
-  </si>
-  <si>
-    <t>12/21/2024 Added UnderPass to htb list</t>
-  </si>
-  <si>
-    <t>UpDown</t>
-  </si>
-  <si>
-    <t>Swagshop</t>
-  </si>
-  <si>
-    <t>Nineveh</t>
-  </si>
-  <si>
-    <t>Pandora</t>
-  </si>
-  <si>
-    <t>OpenAdmin</t>
-  </si>
-  <si>
-    <t>Precious</t>
-  </si>
-  <si>
-    <t>Busqueda</t>
-  </si>
-  <si>
-    <t>Monitored</t>
-  </si>
-  <si>
-    <t>BoardLight</t>
-  </si>
-  <si>
-    <t>Magic</t>
-  </si>
-  <si>
-    <t>Help</t>
-  </si>
-  <si>
-    <t>Editorial</t>
-  </si>
-  <si>
-    <t>Builder</t>
-  </si>
-  <si>
-    <t>Linkvortex</t>
-  </si>
-  <si>
-    <t>UnderPass</t>
-  </si>
-  <si>
-    <t>Proving Grounds Practice</t>
-  </si>
-  <si>
-    <t>Virtual Hacking Labs</t>
-  </si>
-  <si>
-    <t>The real OSCP like boxes, this is just a list with the ones that are best practice and removing the overly complicated ones that are too out of scope and those that were boxes meant to be mostly for OSEP and OSED (example Kyoto and Nara) that were in TJNull list plus adding some new ones</t>
-  </si>
-  <si>
-    <t>Very under rated platform with very OSCP like machines, people that have used it really recommend it for OSCP including me. It has been very crucial help for those that have failed attempts to be able to pass and they are good practice for standalones. Note: seems some lab purchase options are currently out of stock</t>
-  </si>
-  <si>
-    <t>Windows Active Directory</t>
-  </si>
-  <si>
-    <t>ClamAV</t>
-  </si>
-  <si>
-    <t>Kevin</t>
-  </si>
-  <si>
-    <t>Techblog</t>
-  </si>
-  <si>
-    <t>Steven</t>
-  </si>
-  <si>
-    <t>Pelican</t>
-  </si>
-  <si>
-    <t>Resourced</t>
-  </si>
-  <si>
-    <t>Backupadmin V2</t>
-  </si>
-  <si>
-    <t>Aaron</t>
-  </si>
-  <si>
-    <t>Payday</t>
-  </si>
-  <si>
-    <t>Algernon</t>
-  </si>
-  <si>
-    <t>Nagoya</t>
-  </si>
-  <si>
-    <t>Web01-Dev V2</t>
-  </si>
-  <si>
-    <t>Anthony</t>
-  </si>
-  <si>
-    <t>Snookums</t>
-  </si>
-  <si>
-    <t>Jacko</t>
-  </si>
-  <si>
-    <t>Hokkaido</t>
-  </si>
-  <si>
-    <t>Web01-Prd V2</t>
-  </si>
-  <si>
-    <t>Jennifer</t>
-  </si>
-  <si>
-    <t>Bratarina</t>
-  </si>
-  <si>
-    <t>Craft</t>
-  </si>
-  <si>
-    <t>Hutch</t>
-  </si>
-  <si>
-    <t>Forum</t>
-  </si>
-  <si>
-    <t>WinAS01</t>
-  </si>
-  <si>
-    <t>Pebbles</t>
-  </si>
-  <si>
-    <t>Squid</t>
-  </si>
-  <si>
-    <t>Vault</t>
-  </si>
-  <si>
-    <t>Quick</t>
-  </si>
-  <si>
-    <t>AS45</t>
-  </si>
-  <si>
-    <t>Nickel</t>
-  </si>
-  <si>
-    <t>Tiki</t>
-  </si>
-  <si>
-    <t>Trace</t>
-  </si>
-  <si>
-    <t>Hetemit</t>
-  </si>
-  <si>
-    <t>MedJed</t>
-  </si>
-  <si>
-    <t>Helpdesk V2</t>
-  </si>
-  <si>
-    <t>React</t>
-  </si>
-  <si>
-    <t>ZenPhoto</t>
-  </si>
-  <si>
-    <t>Billyboss</t>
-  </si>
-  <si>
-    <t>VPS1723 V2</t>
-  </si>
-  <si>
-    <t>Nukem</t>
-  </si>
-  <si>
-    <t>Shenzi</t>
-  </si>
-  <si>
-    <t>CMS02 V2</t>
-  </si>
-  <si>
-    <t>Cockpit</t>
-  </si>
-  <si>
-    <t>AuthBy</t>
-  </si>
-  <si>
-    <t>Records</t>
-  </si>
-  <si>
-    <t>PyLoader</t>
-  </si>
-  <si>
-    <t>Slort</t>
-  </si>
-  <si>
-    <t>Trails</t>
-  </si>
-  <si>
-    <t>Clue</t>
-  </si>
-  <si>
-    <t>Hepet</t>
-  </si>
-  <si>
-    <t>Dolphin V2</t>
-  </si>
-  <si>
-    <t>Extplorer</t>
-  </si>
-  <si>
-    <t>DVR4</t>
-  </si>
-  <si>
-    <t>Crash</t>
-  </si>
-  <si>
-    <t>Postfish</t>
-  </si>
-  <si>
-    <t>Natural</t>
-  </si>
-  <si>
-    <t>Hawat</t>
-  </si>
-  <si>
-    <t>Mantis</t>
-  </si>
-  <si>
-    <t>Walla</t>
-  </si>
-  <si>
-    <t>Fed V2</t>
-  </si>
-  <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <t>CMS01</t>
-  </si>
-  <si>
-    <t>Apex</t>
-  </si>
-  <si>
-    <t>Tracking</t>
-  </si>
-  <si>
-    <t>Sorcerer</t>
-  </si>
-  <si>
-    <t>JS01</t>
-  </si>
-  <si>
-    <t>Sybaris</t>
-  </si>
-  <si>
-    <t>PBX</t>
-  </si>
-  <si>
-    <t>Peppo</t>
-  </si>
-  <si>
-    <t>Code V2</t>
-  </si>
-  <si>
-    <t>Hunit</t>
-  </si>
-  <si>
-    <t>Teamspeak</t>
-  </si>
-  <si>
-    <t>Readys</t>
-  </si>
-  <si>
-    <t>CMS101</t>
-  </si>
-  <si>
-    <t>Astronaut</t>
-  </si>
-  <si>
-    <t>FW01</t>
-  </si>
-  <si>
-    <t>Bullybox</t>
-  </si>
-  <si>
-    <t>Core</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>Websrv01</t>
-  </si>
-  <si>
-    <t>Exfiltrated</t>
-  </si>
-  <si>
-    <t>Mon02</t>
-  </si>
-  <si>
-    <t>Fanatastic</t>
-  </si>
-  <si>
-    <t>Graphs01</t>
-  </si>
-  <si>
-    <t>QuackerJack</t>
-  </si>
-  <si>
-    <t>PM V2</t>
-  </si>
-  <si>
-    <t>Wombo</t>
-  </si>
-  <si>
-    <t>Tracker</t>
-  </si>
-  <si>
-    <t>Flu</t>
-  </si>
-  <si>
-    <t>Roquefort</t>
-  </si>
-  <si>
-    <t>Levram</t>
-  </si>
-  <si>
-    <t>Mzeeav</t>
-  </si>
-  <si>
-    <t>LaVita</t>
-  </si>
-  <si>
-    <t>Xposedapi</t>
-  </si>
-  <si>
-    <t>Zipper</t>
-  </si>
-  <si>
-    <t>Ochima</t>
-  </si>
-  <si>
-    <t>Fired</t>
-  </si>
-  <si>
-    <t>Scrutiny</t>
-  </si>
-  <si>
-    <t>SPX</t>
-  </si>
-  <si>
-    <t>Vmdak</t>
-  </si>
-  <si>
-    <t>Proving Grounds Play</t>
-  </si>
-  <si>
-    <t>Mostly boxes from vulnhub hosted by offsec for free</t>
-  </si>
-  <si>
-    <t>Platform with realistic scenarios, really good for learning Windows and AD exploitation.</t>
-  </si>
-  <si>
-    <t>Amaterasu</t>
-  </si>
-  <si>
-    <t>Sync</t>
-  </si>
-  <si>
-    <t>Baby</t>
-  </si>
-  <si>
-    <t>Loly</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Job</t>
-  </si>
-  <si>
-    <t>Baby2</t>
-  </si>
-  <si>
-    <t>Potato</t>
-  </si>
-  <si>
-    <t>Build</t>
-  </si>
-  <si>
-    <t>Job2</t>
-  </si>
-  <si>
-    <t>Breach</t>
-  </si>
-  <si>
-    <t>Stapler</t>
-  </si>
-  <si>
-    <t>Phantom</t>
-  </si>
-  <si>
-    <t>BBScute</t>
-  </si>
-  <si>
-    <t>Sweep</t>
-  </si>
-  <si>
-    <t>Gaara</t>
-  </si>
-  <si>
-    <t>Blogger</t>
-  </si>
-  <si>
-    <t>Chains:</t>
-  </si>
-  <si>
-    <t>FunboxEasyEnum</t>
-  </si>
-  <si>
-    <t>Trusted</t>
-  </si>
-  <si>
-    <t>Reflection</t>
-  </si>
-  <si>
-    <t>Hybrid</t>
-  </si>
-  <si>
-    <t>Lustrous</t>
-  </si>
-  <si>
-    <t>VulnLab</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
@@ -1273,6 +1275,87 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1323,87 +1406,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1684,7 +1686,7 @@
   <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1700,208 +1702,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="55"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="58"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="58"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:9" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="63" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:9" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="40" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33"/>
     </row>
     <row r="5" spans="1:9" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="40" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="42"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="42"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="42"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="50"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="42"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="33"/>
     </row>
     <row r="9" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="42"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
     </row>
     <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="42"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="42"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="33"/>
     </row>
     <row r="12" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="48"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="43"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="60"/>
     </row>
     <row r="14" spans="1:9" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="29"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="63"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="49"/>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1946,128 +1948,128 @@
       <c r="F17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="H17" s="14" t="s">
         <v>29</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>30</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="C18" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="H18" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="G19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="H19" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>44</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="G20" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="H20" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="14"/>
@@ -2075,107 +2077,107 @@
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="H23" s="14"/>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="H24" s="14"/>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="H25" s="14"/>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="H26" s="14"/>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="1"/>
       <c r="E27" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
@@ -2184,17 +2186,17 @@
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
@@ -2203,17 +2205,17 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
@@ -2222,17 +2224,17 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
@@ -2241,15 +2243,15 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="1"/>
       <c r="E31" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
@@ -2258,15 +2260,15 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="1"/>
       <c r="E32" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
@@ -2275,17 +2277,17 @@
     </row>
     <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -2294,15 +2296,15 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F34" s="18"/>
       <c r="G34" s="1"/>
@@ -2311,15 +2313,15 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="1"/>
@@ -2328,13 +2330,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
       <c r="D36" s="1"/>
       <c r="E36" s="17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -2343,13 +2345,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
       <c r="D37" s="1"/>
       <c r="E37" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F37" s="18"/>
       <c r="G37" s="1"/>
@@ -2358,13 +2360,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38" s="1"/>
       <c r="E38" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -2373,7 +2375,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
@@ -2386,7 +2388,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
@@ -2399,7 +2401,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
@@ -2412,7 +2414,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
@@ -2425,7 +2427,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
@@ -2438,7 +2440,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
@@ -2451,7 +2453,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
@@ -2464,7 +2466,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="8"/>
@@ -2477,7 +2479,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
@@ -2490,7 +2492,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="8"/>
@@ -2503,7 +2505,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="8"/>
@@ -2516,7 +2518,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
@@ -2529,7 +2531,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
@@ -2542,7 +2544,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
@@ -2555,7 +2557,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="8"/>
@@ -2578,32 +2580,32 @@
       <c r="I54" s="1"/>
     </row>
     <row r="55" spans="1:9" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A55" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="B55" s="28"/>
-      <c r="C55" s="29"/>
+      <c r="A55" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" s="55"/>
+      <c r="C55" s="56"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="F55" s="28"/>
-      <c r="G55" s="29"/>
+      <c r="E55" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="F55" s="55"/>
+      <c r="G55" s="56"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
     <row r="56" spans="1:9" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="22"/>
+      <c r="A56" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" s="48"/>
+      <c r="C56" s="49"/>
       <c r="D56" s="10"/>
-      <c r="E56" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="F56" s="21"/>
-      <c r="G56" s="22"/>
+      <c r="E56" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="F56" s="48"/>
+      <c r="G56" s="49"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
@@ -2615,7 +2617,7 @@
         <v>21</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="3" t="s">
@@ -2630,20 +2632,20 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G58" s="16"/>
       <c r="H58" s="1"/>
@@ -2651,20 +2653,20 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G59" s="16"/>
       <c r="H59" s="1"/>
@@ -2672,20 +2674,20 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>153</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G60" s="16"/>
       <c r="H60" s="1"/>
@@ -2693,20 +2695,20 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G61" s="16"/>
       <c r="H61" s="1"/>
@@ -2714,20 +2716,20 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>163</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G62" s="16"/>
       <c r="H62" s="1"/>
@@ -2735,20 +2737,20 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>168</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G63" s="16"/>
       <c r="H63" s="1"/>
@@ -2756,18 +2758,18 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="1"/>
       <c r="E64" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G64" s="16"/>
       <c r="H64" s="1"/>
@@ -2775,18 +2777,18 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="1"/>
       <c r="E65" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G65" s="16"/>
       <c r="H65" s="1"/>
@@ -2794,15 +2796,15 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="1"/>
       <c r="E66" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="16"/>
@@ -2811,15 +2813,15 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="1"/>
       <c r="E67" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="16"/>
@@ -2828,15 +2830,15 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="1"/>
       <c r="E68" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="16"/>
@@ -2845,15 +2847,15 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="1"/>
       <c r="E69" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="1"/>
@@ -2862,15 +2864,15 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="1"/>
       <c r="E70" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="1"/>
@@ -2879,15 +2881,15 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="1"/>
       <c r="E71" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="1"/>
@@ -2896,13 +2898,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
       <c r="D72" s="1"/>
       <c r="E72" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F72" s="7"/>
       <c r="G72" s="1"/>
@@ -2911,13 +2913,13 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="8"/>
       <c r="D73" s="1"/>
       <c r="E73" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F73" s="7"/>
       <c r="G73" s="1"/>
@@ -2926,13 +2928,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
       <c r="D74" s="1"/>
       <c r="E74" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="1"/>
@@ -2941,13 +2943,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="8"/>
       <c r="D75" s="1"/>
       <c r="E75" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="1"/>
@@ -2956,13 +2958,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
       <c r="D76" s="1"/>
       <c r="E76" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="1"/>
@@ -2971,13 +2973,13 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="8"/>
       <c r="D77" s="1"/>
       <c r="E77" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="1"/>
@@ -2986,13 +2988,13 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
       <c r="D78" s="1"/>
       <c r="E78" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="1"/>
@@ -3001,13 +3003,13 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
       <c r="D79" s="1"/>
       <c r="E79" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="1"/>
@@ -3016,13 +3018,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
       <c r="D80" s="1"/>
       <c r="E80" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="1"/>
@@ -3031,13 +3033,13 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
       <c r="D81" s="1"/>
       <c r="E81" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="1"/>
@@ -3046,13 +3048,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
       <c r="D82" s="1"/>
       <c r="E82" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="1"/>
@@ -3061,13 +3063,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
       <c r="D83" s="1"/>
       <c r="E83" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="1"/>
@@ -3076,13 +3078,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
       <c r="D84" s="1"/>
       <c r="E84" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="1"/>
@@ -3091,13 +3093,13 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="8"/>
       <c r="D85" s="1"/>
       <c r="E85" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="1"/>
@@ -3106,13 +3108,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
       <c r="D86" s="1"/>
       <c r="E86" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F86" s="7"/>
       <c r="G86" s="1"/>
@@ -3121,13 +3123,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B87" s="7"/>
       <c r="C87" s="8"/>
       <c r="D87" s="1"/>
       <c r="E87" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="1"/>
@@ -3136,13 +3138,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="8"/>
       <c r="D88" s="1"/>
       <c r="E88" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F88" s="7"/>
       <c r="G88" s="1"/>
@@ -3151,7 +3153,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="8"/>
@@ -3164,7 +3166,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="8"/>
@@ -3177,7 +3179,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B91" s="7"/>
       <c r="C91" s="8"/>
@@ -3190,7 +3192,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B92" s="7"/>
       <c r="C92" s="8"/>
@@ -3203,7 +3205,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B93" s="7"/>
       <c r="C93" s="8"/>
@@ -3216,7 +3218,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B94" s="7"/>
       <c r="C94" s="8"/>
@@ -3229,7 +3231,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B95" s="7"/>
       <c r="C95" s="8"/>
@@ -3242,7 +3244,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
@@ -3255,7 +3257,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="8"/>
@@ -3268,7 +3270,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B98" s="7"/>
       <c r="C98" s="8"/>
@@ -3281,7 +3283,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="8"/>
@@ -3294,7 +3296,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B100" s="7"/>
       <c r="C100" s="8"/>
@@ -3307,7 +3309,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="8"/>
@@ -3330,32 +3332,32 @@
       <c r="I102" s="1"/>
     </row>
     <row r="103" spans="1:9" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A103" s="27" t="s">
-        <v>242</v>
-      </c>
-      <c r="B103" s="28"/>
-      <c r="C103" s="29"/>
+      <c r="A103" s="54" t="s">
+        <v>240</v>
+      </c>
+      <c r="B103" s="55"/>
+      <c r="C103" s="56"/>
       <c r="D103" s="1"/>
-      <c r="E103" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="F103" s="28"/>
-      <c r="G103" s="29"/>
+      <c r="E103" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="F103" s="55"/>
+      <c r="G103" s="56"/>
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
     </row>
     <row r="104" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="B104" s="21"/>
-      <c r="C104" s="22"/>
+      <c r="A104" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="B104" s="48"/>
+      <c r="C104" s="49"/>
       <c r="D104" s="1"/>
-      <c r="E104" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="F104" s="21"/>
-      <c r="G104" s="22"/>
+      <c r="E104" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="F104" s="48"/>
+      <c r="G104" s="49"/>
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
     </row>
@@ -3380,64 +3382,64 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G106" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H106" s="1"/>
       <c r="I106" s="1"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="G107" s="8" t="s">
         <v>249</v>
-      </c>
-      <c r="F107" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="G107" s="8" t="s">
-        <v>251</v>
       </c>
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="G108" s="8" t="s">
         <v>253</v>
-      </c>
-      <c r="F108" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="G108" s="8" t="s">
-        <v>255</v>
       </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3445,14 +3447,14 @@
       <c r="E109" s="6"/>
       <c r="F109" s="7"/>
       <c r="G109" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H109" s="1"/>
       <c r="I109" s="1"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3460,14 +3462,14 @@
       <c r="E110" s="6"/>
       <c r="F110" s="7"/>
       <c r="G110" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H110" s="1"/>
       <c r="I110" s="1"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3480,7 +3482,7 @@
     </row>
     <row r="112" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3488,14 +3490,14 @@
       <c r="E112" s="6"/>
       <c r="F112" s="7"/>
       <c r="G112" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H112" s="1"/>
       <c r="I112" s="1"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3503,7 +3505,7 @@
       <c r="E113" s="6"/>
       <c r="F113" s="7"/>
       <c r="G113" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H113" s="1"/>
       <c r="I113" s="1"/>
@@ -3516,7 +3518,7 @@
       <c r="E114" s="6"/>
       <c r="F114" s="7"/>
       <c r="G114" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H114" s="1"/>
       <c r="I114" s="1"/>
@@ -3529,7 +3531,7 @@
       <c r="E115" s="6"/>
       <c r="F115" s="7"/>
       <c r="G115" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H115" s="1"/>
       <c r="I115" s="1"/>
@@ -3542,32 +3544,11 @@
       <c r="E116" s="6"/>
       <c r="F116" s="7"/>
       <c r="G116" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F9:I9"/>
     <mergeCell ref="A104:C104"/>
     <mergeCell ref="E104:G104"/>
     <mergeCell ref="E3:E12"/>
@@ -3584,6 +3565,27 @@
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="F10:I10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:I3"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>

</xml_diff>